<commit_message>
Update outputfile subdirectory names to reflect the current figure organization
</commit_message>
<xml_diff>
--- a/Source_Data_Fig_4.xlsx
+++ b/Source_Data_Fig_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmansour/Desktop/DropletDeformationPaper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielmansour/Documents/GitHub/abp-deformable-droplet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0928DE02-99D2-B644-A22D-1A4F9638BBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAB0FD9-F93D-7B44-8C41-88009F465301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" xr2:uid="{5F0BFDA7-77F2-F445-9194-E20F0C59AABD}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Aspect Ratio</t>
   </si>
@@ -80,6 +80,18 @@
   </si>
   <si>
     <t>CapZ Concentration</t>
+  </si>
+  <si>
+    <t>0.0 µM</t>
+  </si>
+  <si>
+    <t>0.5 µM</t>
+  </si>
+  <si>
+    <t>1.0 µM</t>
+  </si>
+  <si>
+    <t>2.0 µM</t>
   </si>
 </sst>
 </file>
@@ -575,7 +587,7 @@
   <dimension ref="A1:U475"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,17 +773,17 @@
       <c r="O5">
         <v>1.028</v>
       </c>
-      <c r="R5" s="4">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="T5" s="4">
-        <v>1</v>
-      </c>
-      <c r="U5" s="4">
-        <v>2</v>
+      <c r="R5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -11684,7 +11696,7 @@
   <dimension ref="A1:U475"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11870,17 +11882,17 @@
       <c r="O5">
         <v>1.028</v>
       </c>
-      <c r="R5" s="4">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="T5" s="4">
-        <v>1</v>
-      </c>
-      <c r="U5" s="4">
-        <v>2</v>
+      <c r="R5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>